<commit_message>
Update User Class [Edit user]
</commit_message>
<xml_diff>
--- a/build/classes/db/Administrator.xlsx
+++ b/build/classes/db/Administrator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Redzer0\Desktop\iHotel\src\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F063D5-A0E8-4D45-A181-3D4A4BFDF9EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908BFAF8-17F4-46F5-879A-DBCF3566EC68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4845" yWindow="2895" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="2430" windowWidth="8625" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Administrator" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>ID</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>redzenova123</t>
+  </si>
+  <si>
+    <t>admin</t>
   </si>
 </sst>
 </file>
@@ -386,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,6 +424,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>